<commit_message>
Finish the function part of transforming from excel to excel.
Signed-off-by: Spark-Liang <369453502@qq.com>
</commit_message>
<xml_diff>
--- a/test/xl_transform/main_test/test_data/TestFromExcelToExcel/Result.xlsx
+++ b/test/xl_transform/main_test/test_data/TestFromExcelToExcel/Result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestOut1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy\-m\-d"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,14 +158,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -451,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -546,9 +540,6 @@
         <v>12.35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="2"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -559,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
1. Make the framework to be compatible to python 2.7.x .
</commit_message>
<xml_diff>
--- a/test/xl_transform/main_test/test_data/TestFromExcelToExcel/Result.xlsx
+++ b/test/xl_transform/main_test/test_data/TestFromExcelToExcel/Result.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\ProjectData\ExcelTransformer\test\xl_transform\main_test\test_data\TestFromExcelToExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Spark\Python\ProjectData\ExcelTransformer\test\xl_transform\main_test\test_data\TestFromExcelToExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="TestOut1" sheetId="1" r:id="rId1"/>
@@ -25,41 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>2019-12-20</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>2019-12-21</t>
-  </si>
-  <si>
     <t>0.656070049</t>
   </si>
   <si>
-    <t>-30</t>
-  </si>
-  <si>
-    <t>0.885854449</t>
-  </si>
-  <si>
-    <t>2019-12-22</t>
-  </si>
-  <si>
     <t>-0.344592265</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>-0.027395487</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -88,49 +64,29 @@
   </si>
   <si>
     <t>decimal_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>40.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2020-01-01 09:04:01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019-12-31 09:04:01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019-12-31 12:23:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-10.00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -158,16 +114,28 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -447,102 +415,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2">
+        <v>43830.515972222223</v>
+      </c>
+      <c r="B2" s="3">
+        <v>43819</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="4">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4">
+        <v>40</v>
+      </c>
+      <c r="F2" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2">
+        <v>43830.377789351849</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43820</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="4">
+        <v>-30</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.88585444899999999</v>
+      </c>
+      <c r="F3" s="5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
+        <v>43831.377789351849</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43821</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-2.7395487E-2</v>
+      </c>
+      <c r="F4" s="5">
         <v>12.35</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -550,27 +519,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>5.01</v>
       </c>
@@ -584,7 +553,7 @@
         <v>5.42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>9.92</v>
       </c>
@@ -598,7 +567,7 @@
         <v>7.51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4.22</v>
       </c>
@@ -612,7 +581,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3.99</v>
       </c>
@@ -629,5 +598,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>